<commit_message>
UPDATE robot.db and resources
</commit_message>
<xml_diff>
--- a/resources/suplementos_deportivos.xlsx
+++ b/resources/suplementos_deportivos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacio\RocketbotProjects\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159843A5-3B15-493E-BC9E-1699CF8D2AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA5BBF3-926E-4366-A840-AABF40250EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{ED8A9987-28D5-47DF-8389-886DA2FF1942}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{4C684BF5-D5C3-4217-808F-4412D93DA393}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
   <si>
     <t>id</t>
   </si>
@@ -57,46 +57,49 @@
     <t>whey protein</t>
   </si>
   <si>
+    <t>Suplemento En Polvo Star Nutrition Platinum Whey Protein Chocolate Suizo Pote 908g Vaso Legend 600ml</t>
+  </si>
+  <si>
+    <t>10% OFF</t>
+  </si>
+  <si>
+    <t>https://click1.mercadolibre.com.ar/mclics/clicks/external/MLA/count?a=036FoO9y9NH58s%2FLxVhPxfRraW%2FvMyC2j%2BXU5ACJckr9GupyKmwpOYeMGwrAqpqzG2PPwB%2FvqQ%2B4R8%2FbvVeUNDU5WYZvV2XGpv3LBbKUzg9qw9hOA0BGZtMbHg8HgABM%2BazKoq1s0Y7ohO6VLqh6%2F72q4OqZlhkuPgdst4O9LyrB99EHWD6CUlq82xE0Gp80BFMB7%2B9fl2p7EWWSH12CCPfJK4jqnVxwnkENtWi9bP6kZDLcVCfVzHuws99U8P4pXO6G4iz9xSpJ1cWCGtEhTBL8CVSwa1LP8R0%2BxlnuEAHamxIBc8Lse%2FjEtOeFcx5hO0MzbUw3pe6Bjk61okDxFifDx5VvM8I96KLno3Lj4eeqcThsidmVxK0l6Ds7o%2BfkmpyJDRNlL8Urr8zmr%2B2ErYUA0l5nnDFD7yqAeoxdIKFVEfMFr5n%2FS8VqrlNjWyGS4Swj8I7U%2B7%2Bxr6GJsUtWEhVHhIdB9sKKCnWZaNep6xtHG0dkVY%2BNgyCtXWLbU2UDl%2F8ymg08BNsw8lpgSIwiuht4je3K50yvnawrGAaUmLHt85BLhWz9Cw%2B8o7gHIwRW93ilwV%2Bp5y84CNZFIMFb0TfVtZvKiSFLTmR27RuDDqDMvbPSu2n346hhJ1928FVAjVTR7pQIh75MgIRMooc6FGfqcWlucKUXKlWm5LL1dDi20BTrqUi45lPJVw9lby3rzteEffB0%2BQat4H8nNPr9T1p1rswr1wAcku5IXcv6dNZTZeRYnOyecHAaq2dDESy7TQD%2BBdOrSAPYZ2D1CfNqz3qgmQl1psRz%2BScqLqZqw4PY14s3zc34eiHKwPxYjVsNugGEduvP4FTxHYSsP0HkmG%2Fgp2NvmIdMq6HbqFYEhJV4UVz%2BY70vUVfzTBXWoo2xe06G17VBkHLiZFDOcpAFEHEwG2JVoTrFpuWec45HyPxKzxSdBiX1k1Ji0cf7u7M%3D&amp;e=mclics%2Fadvertising-results-augmenter-on%2B15097%2Cmclics%2Fmin-budget-throttling%2B54896%2Cmclics%2Fdiscard-bid-lt-min%2B45363%2Cmclics%2Fdynamic-yield-factor%2B73919%2Cmclics%2Fmore-ads-migration%2B56865%2Cmclics%2Fmax-bid-capped%2B36382%2Cmclics%2Fmax-bid-item-factor%2B23927%2Cmclics%2Fdomain-rules-override%2B74278%2Cmclics%2Fgmv-predictor%2B52393%2Cmclics%2Foverride-min-seasonality%2B49092&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=57b44c48-d918-4718-a181-ef7677647573&amp;wid=MLA1896368696&amp;sid=search</t>
+  </si>
+  <si>
+    <t>Suplemento en Polvo Star Nutrition Platinum Whey Protein Sabor Chocolate Suizo en Sachet de 3kg</t>
+  </si>
+  <si>
+    <t>https://click1.mercadolibre.com.ar/mclics/clicks/external/MLA/count?a=2Ux%2FqVjvwHKkyA4WKyO9yLspj%2F%2BD8BkE34mGhkpTCTJPwGHxFsB8Utfr6HaDoAHCaKygPQNBspBwxnRsve2W2jnbOBg2ADpAYOjFpYTKFwEne%2Bn4jMEstyJ1BD6OGj7jbxdNTvQhbGZdfpznauJA8ks7UWQLVuVYTVsiQgOFV9bF0NBoyY3mw7MI31GCOs%2FP2L%2BypMDFuMm9M%2Btfg4dOdhTGUUlxFF8GNIEPAdyq18es8C%2Bxo%2BYzLHvGrMHKejp0CEM9n6HDKQ88bQ45GS4xmnl2DmiUwAjJb96y02grv2eH6mYQ7Pp%2F6wxX%2Fl3r79wTFShkKvbPttsIjmncnEQJJtO74EixPcTCzFTDznc56i5BwjaEZHpQtR9Ggk8QrHpQIMu921aM4mgd4UOifzwlJRlkA%2BQTAdjzjJ7aSqQ%2Bh4RjVhLgT8EXwXlLUnbRMXj3yvKStk%2FL8XvMpW8L67tD9qdp3OfqkOi1%2FYKyqzPuJ2peoVFPc0jAjyxtUTPpzmUhdFVr%2Fi5eYO8XKQjfjNf8EntFX7opfL%2Bqiq8bqVJpERLaQGUOzUhw4WNNgoLAGktGaWyPRT0H3JYq4lrh7LzO9%2FSP4%2B8oBWehT25VDjI5bD7RWatXmYtduF55406acUIaDONkcV048i2cQTu%2BA%2FVTblfEsuBSV8i8NMtr5NqXqcygcwli3YDSU1pQhwJ2auMqXGZavzMHUVxUxc7ZWOFnkfVbJ3mo%2B26XmLEIGSh3aNua20F4LKwAIqFcvFMwjXdi80Qm7kuvlz%2BWvuhtQJuNmmyQmC6tzcm4LjBrdDeeG6CemSHeRsz9MTISSBzq%2F1LpNoz8fmVmyxg6mc%2ByplqBwUHYWGSK4IFp1F23DjpVgIZ8P1dpnvV7puKdZ0CZgWobFodncJJVz5jTgUHyJF7aqeEZM80Ab%2FoW3H5o6vAAsEtlia1FIrEjMQ%3D%3D&amp;e=mclics%2Fadvertising-results-augmenter-on%2B15097%2Cmclics%2Fmin-budget-throttling%2B54896%2Cmclics%2Fdiscard-bid-lt-min%2B45363%2Cmclics%2Fdynamic-yield-factor%2B73919%2Cmclics%2Fmore-ads-migration%2B56865%2Cmclics%2Fmax-bid-capped%2B36382%2Cmclics%2Fmax-bid-item-factor%2B23927%2Cmclics%2Fdomain-rules-override%2B74278%2Cmclics%2Fgmv-predictor%2B52393%2Cmclics%2Foverride-min-seasonality%2B49092&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=57b44c48-d918-4718-a181-ef7677647573&amp;wid=MLA1485878848&amp;sid=search</t>
+  </si>
+  <si>
+    <t>Suplemento en polvo ENA Sport True Made Whey Protein proteínas sabor vanilla ice cream en pote de 930g</t>
+  </si>
+  <si>
+    <t>15% OFF</t>
+  </si>
+  <si>
+    <t>https://www.mercadolibre.com.ar/suplemento-en-polvo-ena-sport-true-made-whey-protein-proteinas-sabor-vanilla-ice-cream-en-pote-de-930g/p/MLA14287435#polycard_client=search-nordic&amp;searchVariation=MLA14287435&amp;wid=MLA1385729149&amp;position=3&amp;search_layout=stack&amp;type=product&amp;tracking_id=57b44c48-d918-4718-a181-ef7677647573&amp;sid=search</t>
+  </si>
+  <si>
+    <t>Suplemento en polvo ENA Sport True Made proteínas sabor double rich chocolate en pote de 930g</t>
+  </si>
+  <si>
+    <t>https://www.mercadolibre.com.ar/suplemento-en-polvo-ena-sport-true-made-proteinas-sabor-double-rich-chocolate-en-pote-de-930g/p/MLA14287437#polycard_client=search-nordic&amp;searchVariation=MLA14287437&amp;wid=MLA1116976337&amp;position=5&amp;search_layout=stack&amp;type=product&amp;tracking_id=57b44c48-d918-4718-a181-ef7677647573&amp;sid=search</t>
+  </si>
+  <si>
     <t>Star Nutrition Whey Protein 908g Sabor Chocolate suizo Doypack En Polvo</t>
   </si>
   <si>
-    <t>10% OFF</t>
-  </si>
-  <si>
-    <t>https://click1.mercadolibre.com.ar/mclics/clicks/external/MLA/count?a=4Xli08I4SaMxrneXm%2Bb%2Fhb5V4J2TlW9ZnS6T6c4mZBGjwHn7mvcMyzcZt%2B8HBbtpGxbj0kakCu9HbJXTPPzL65WyAM0qK2Hpag%2BH0m9drOUJ6408Oj3Xp8lVUB%2F4WOf2hDRvF8fXZqpx6p0nYxJeS3V%2BuTVjkkZk%2FmP%2FICvZGn8FAZb5z%2FFzyfpke3HXsDCwGXRoU99RaZLIQ7X5cHnEj0mBSHn63DiifuR9tClQm7qoZxlKWzuDTyH8qaxi8vBcm0zekZCim1eOM%2BeasTOa2vV6ORG1dKcOdlsKYJJmeNe8h248VY9d2jG7BQZqJmxOguMaYpyPCkbfFK1mNngOHgvBwPaxVvQ1UecwuWpOsAs1lPO%2Fh%2BZpI%2BenGZhKHwIh2IE1c3Di%2BhfkBdKahG04hsMtEMo5IUIlid8dvgSh4D4XA4yNrCxuwxKUohLc9dVwtJ1kwV3EGhFsLhgfISww7m8lpIspURXUvT5JE5ytDiK8auGSlaxBL9FugCOYs21JQ3ouLQ6%2BAbLFTh8S8D38g9G6l14gCZeBckQVAWUsKgJnWaqyjWUNX46RtlwYi%2BcDOPHKidsNYRZh%2BD4S6Pnczu1NfPAnniMhUuC0rczAIPTJfXW7yl9HZDhfDexcKs7VCSnlvmlmOM4sPfkVUjswqbyTzWTGyatNdJuO8moZIboO1k33B02%2FO2uVcbkWRjdd4wlfL3IR8DlrcRcWEMPHm7X0Ad5Zy1WokhVVNN2Xu6A7pcigE%2F1EbtQh%2FNx16oUC35imSMT%2Fkw%2FxGVBH%2F%2BkCSMhDTNaWVRCjF6q9K1se%2BpkOm5ChxxC5%2FP6O9Nw0EZtzirHqoGgrkw5D7EQn0SNXihA342ZkcvFwosmgUtARc%2BsWpz2GXiDyg%2FUadzAkNtXoI110EH9rs4VgyBFEd6hJ0WiG&amp;e=mclics%2Fadvertising-results-augmenter-on%2B15097%2Cmclics%2Fmin-budget-throttling%2B54896%2Cmclics%2Fdiscard-bid-lt-min%2B45363%2Cmclics%2Fdynamic-yield-factor%2B73919%2Cmclics%2Fmore-ads-migration%2B56865%2Cmclics%2Fmax-bid-capped%2B36382%2Cmclics%2Fmax-bid-item-factor%2B23927%2Cmclics%2Fdomain-rules-override%2B74278%2Cmclics%2Fgmv-predictor%2B52393%2Cmclics%2Foverride-min-seasonality%2B49092&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=434de1aa-7e52-46b7-bfd3-877f93b2f905&amp;wid=MLA1367282777&amp;sid=search</t>
-  </si>
-  <si>
-    <t>Suplemento En Polvo Star Nutrition Platinum Whey Protein Chocolate Suizo Pote 908g Vaso Legend 600ml</t>
-  </si>
-  <si>
-    <t>https://click1.mercadolibre.com.ar/mclics/clicks/external/MLA/count?a=8RIG5tHHN8IwYbzE8t3tv778SaKPSth8k%2Fq2jbK63KdKUUxKuAs56pita54nNZFc1B6PgGcWWGPwcUWOdMCkqGVXTj6WjYeiQWbDAshiXnlC8i4mnsidYr6hLvWbvBG2gU%2BipI0MvCaoPFVTPMsM42lbrNkiCe9jG72SITRfno%2Fw7BQvEoT70UwntOJuPXrmDFXgqoaf%2FtCweMrkoVvSr33s8hRWsjFIwwNzcdKuqXg2P8ioPw%2BbzKAoq4LF62fKxAev2JXKHcdz41B%2Baw7KYx%2FwDCvVhW3rGWse1eoJpZ0stxVjBaaIP2Arw0%2BmORwo2yQGRKppBT8xPijFgX%2BghErDuBXkBCzFUcenIFsuPwCNsItn255QF9s4EEHKmNKPjgg55sVnrq53fGMCs2Lid99%2FV57A3wwPu%2F7PNZoT0TMZLmF%2BYpt7tRzq2Qe5kURLC8rYYFsTpMO0bRuqVq%2B4eiSxIIHZHOpyjIUNGvTAndjdJDgM3PktjhX%2FsxDbuH1i%2FdDSEbFeS1P8saDq04PkFGw4hwSzpE1fF9Y4WdsyVItu8T%2BoeWpGeHRxTxBdv1nUIoam6paFpEalw5xyVR5fJRdZuJgxP7CRPRpO3a2ZBGm1u0b1xre71BeClkDxqb3Z2WccNb94Ba3Tz911%2FKUjnZMSd8eu5JoK1dbE2VBwuSXOvH3Oguzsojig2GZeBLe9UL0Dc1w342oXK%2FvVWxiaxir9lN2%2FhaHPIYvSW5u3l1A8%2Bs5EEML3Afb5Ur2bo%2FlU%2FFCIgD6oMlCbj4co%2F9ewvFrZAhG1iR30z0u3Xa0yEwfTPRV9JBaj8p7UsFep3V%2BAEFyUcCD8%2FbDkMhorrZWRnSUahrrCrxUJTiS47GKaaFX%2F%2F9T0%2FdAx8Y8twar4HdfS1CUnA3ciMFku0e5CXDwmdWsczubl%2BierGsHFWPXj3yPuDQQForLWPbKK%2FI6G034%3D&amp;e=mclics%2Fadvertising-results-augmenter-on%2B15097%2Cmclics%2Fmin-budget-throttling%2B54896%2Cmclics%2Fdiscard-bid-lt-min%2B45363%2Cmclics%2Fdynamic-yield-factor%2B73919%2Cmclics%2Fmore-ads-migration%2B56865%2Cmclics%2Fmax-bid-capped%2B36382%2Cmclics%2Fmax-bid-item-factor%2B23927%2Cmclics%2Fdomain-rules-override%2B74278%2Cmclics%2Fgmv-predictor%2B52393%2Cmclics%2Foverride-min-seasonality%2B49092&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=434de1aa-7e52-46b7-bfd3-877f93b2f905&amp;wid=MLA1896368696&amp;sid=search</t>
-  </si>
-  <si>
-    <t>Suplemento en polvo ENA Sport True Made Whey Protein proteínas sabor vanilla ice cream en pote de 930g</t>
-  </si>
-  <si>
-    <t>15% OFF</t>
-  </si>
-  <si>
-    <t>https://www.mercadolibre.com.ar/suplemento-en-polvo-ena-sport-true-made-whey-protein-proteinas-sabor-vanilla-ice-cream-en-pote-de-930g/p/MLA14287435#polycard_client=search-nordic&amp;searchVariation=MLA14287435&amp;wid=MLA1385729149&amp;position=8&amp;search_layout=stack&amp;type=product&amp;tracking_id=434de1aa-7e52-46b7-bfd3-877f93b2f905&amp;sid=search</t>
-  </si>
-  <si>
-    <t>Suplemento en polvo ENA Sport True Made proteínas sabor double rich chocolate en pote de 930g</t>
-  </si>
-  <si>
-    <t>https://www.mercadolibre.com.ar/suplemento-en-polvo-ena-sport-true-made-proteinas-sabor-double-rich-chocolate-en-pote-de-930g/p/MLA14287437#polycard_client=search-nordic&amp;searchVariation=MLA14287437&amp;wid=MLA1116976337&amp;position=12&amp;search_layout=stack&amp;type=product&amp;tracking_id=434de1aa-7e52-46b7-bfd3-877f93b2f905&amp;sid=search</t>
-  </si>
-  <si>
-    <t>16% OFF</t>
-  </si>
-  <si>
-    <t>https://www.mercadolibre.com.ar/star-nutrition-whey-protein-908g-sabor-chocolate-suizo-doypack-en-polvo/p/MLA19544897#polycard_client=search-nordic&amp;searchVariation=MLA19544897&amp;wid=MLA1431943611&amp;position=14&amp;search_layout=stack&amp;type=product&amp;tracking_id=434de1aa-7e52-46b7-bfd3-877f93b2f905&amp;sid=search</t>
-  </si>
-  <si>
-    <t>Suplemento en Polvo Star Nutrition Platinum Whey Protein Sabor Chocolate Suizo en Sachet de 3kg</t>
-  </si>
-  <si>
-    <t>https://click1.mercadolibre.com.ar/mclics/clicks/external/MLA/count?a=RXVIS1TYgLBFzxctf0HgtSMKTIMectOLKJQO0C19dwlCxVgh%2FOzAFAhs44wQArb%2FJXjyFdD0FEZ3iwRyWWgHKTQ9zenctpIKynPOAX6rwPoZv0WAgSPSpdl6tukfBZgz2O3tsdPuv5Ac8a2i8GNFfpLc9e%2FBAqCYUOcqV4H4QT9XAStVKcHMUYF%2FMceUGi%2Bq3Xx8dgnZIxaLF4M38G4DalFup3czofmaLWpKqwSoWU5tvE%2F8gpY0lOZAiIy2f6b%2FmjOgwFCwt3mD3PcEMlvVcNQE%2F4jFxxMF76UTYg3nKeRKzGL3xzoT7df22pBs6IWsSPb68hXFf5mnF%2BOz1eYTsjGQlkIR%2FVZmjFRWabTiLgbTQc09sDHbKUnyY8jYp2C4JiT88rNkC7QJeWL5Dpj1HKcVLq5mhTOHM0eeo8%2Fbd%2Bhuhbiz1ZYdpVvzUUbdiFI0vMBbudNIBW%2BgCQSH1ffFMBdYSTab6V5%2F946DPQjId%2Fi0GW2EwahQyGhUG4OvTM%2BFzdnXjA9BWgv0Np1AddWCmzF0NtUSlkTHOUxbEiJBifNsDGcJoKR%2BEdQy8%2BR9GDZz5Sple99JpOpGql4cojC35B52ZmOSs17G2vTLQ8%2BC7wYWln46QbTfYdenA5O7%2BqiqeNG2NdsQ4twLCvdM40yXi5HPirtqMUDmuCbdHDlUvepAYJFOB0EipZzZs3k2UQvGYOerQjs7qsN%2BF05p9CkRmT%2F6MfGsEa1yHzWadmWWm%2F7887tDa7CnHz%2Fe0tZnovpN9WOo7It7Rh2m2CjdKT93K2AGrg%2FAxPyAT11pvKSEOHBruW5QWMOlMseJYgdbrSvbTIAeTBWlydp23UrKuCJXgOVihdf6i%2FWXcDwM8TJ3XJhtYYfgzk78DHAdHlKXc8Bb6DS%2Fs3rP4mOG4eClilOiW1A%2FHrjtF5GmJXvnXh10VpBZVI2dbNA2NCQ%3D&amp;e=mclics%2Fadvertising-results-augmenter-on%2B15097%2Cmclics%2Fmin-budget-throttling%2B54896%2Cmclics%2Fdiscard-bid-lt-min%2B45363%2Cmclics%2Fdynamic-yield-factor%2B73919%2Cmclics%2Fmore-ads-migration%2B56865%2Cmclics%2Fmax-bid-capped%2B36382%2Cmclics%2Fmax-bid-item-factor%2B23927%2Cmclics%2Fdomain-rules-override%2B74278%2Cmclics%2Fgmv-predictor%2B52393%2Cmclics%2Foverride-min-seasonality%2B49092&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=434de1aa-7e52-46b7-bfd3-877f93b2f905&amp;wid=MLA1485878848&amp;sid=search</t>
+    <t>0% OFF</t>
+  </si>
+  <si>
+    <t>https://www.mercadolibre.com.ar/star-nutrition-whey-protein-908g-sabor-chocolate-suizo-doypack-en-polvo/p/MLA19544897#polycard_client=search-nordic&amp;searchVariation=MLA19544897&amp;wid=MLA1852886938&amp;position=8&amp;search_layout=stack&amp;type=product&amp;tracking_id=57b44c48-d918-4718-a181-ef7677647573&amp;sid=search</t>
+  </si>
+  <si>
+    <t>Suplemento en Polvo Star Nutrition Platinum Whey Protein Sabor Chocolate Suizo en Pote de 908g</t>
+  </si>
+  <si>
+    <t>https://click1.mercadolibre.com.ar/mclics/clicks/external/MLA/count?a=mZYibv2xa7j9TUMpoeSQ34e%2BetdT%2FMrFP%2FHF4k2eT2bGxWuU8IAUigqyjFBlUMKyEdIt368l5geIFs2%2FgRU1viZ3vscSwr0ek7I3GPHWSwtDRfCxdFse7Thla3p2Skaq54QFcdjmexC6r4F7NtEO3upfPJLUHbLt3p7IM1wYeX7qbrB32yuwRLZd%2FI69%2Bwj7rgRurZJT3pe7rCT%2Bl4Wl%2FZX3GRmdUY3hUKkVgu5B%2ByPsKufHUgRFEW%2FlVCT600ttBFRBsDT9n%2BcHMn8%2F1eRBbK2ohLiKa6iQxFQJDJUImzk%2BUT1bSSVxQGW4KncqzkTnLv6ls%2Blzk7IMZJgn9BraIm6AsJX9sbNUl89YDfYDA7bapCW0nrI2ACovu06ADZdiOQqr%2F8gfXfiSPBiYI9A8sUa%2BrKy9RfvRajfkjlh2LTnHevDL81SRCnXLUbITv8gpDkWHxHumw0a7qqdv%2F9G8HU0sGtwjIPBx%2BgBzX1NC4KEKQUT8WKRUH6G5B5vVnOKX7xpTHzi08MQ0C7OngjQuZSxujNyzRzRh%2FwrqU18hfqxV%2B9nI7odwnO5zuNcUD6uEz%2BK7VRAc%2BBa0efUIrun%2Bj5xu4HiuT%2FP%2FFjsJddRMuPNhV7x38dLiabTqk%2FpPUaUHm0dQLS0BYJzeE9EctgFaZDkOFJkzW70weiwpm8jdzv6po2vPpgS9v8evMCT%2FrndLoQgflYoYP67qBKt2Ew7p%2FUeulvN3JeSjKp4gBBKlyv3gUY0dpVi6%2F%2BiSVdTuHAsMuqvEkhhxLMpZz9Q3WGiqv3qNrwT2bzwlb4t9PnBbtfU4wq78u6xxjjk8ve%2FiOzJoR3EGg1ffcHQwUVpmvT43kjR9XDDeIrkqO8t93CSqSTc7cmEdcYdnL2%2BME2bWQUYZB5G9VvqGnJkjcrVIf%2BdQrFrGEjaomUUPjmlVxQUT7Dub%2BJABy7gImw%3D%3D&amp;e=mclics%2Fadvertising-results-augmenter-on%2B15097%2Cmclics%2Fmin-budget-throttling%2B54896%2Cmclics%2Fdiscard-bid-lt-min%2B45363%2Cmclics%2Fdynamic-yield-factor%2B73919%2Cmclics%2Fmore-ads-migration%2B56865%2Cmclics%2Fmax-bid-capped%2B36382%2Cmclics%2Fmax-bid-item-factor%2B23927%2Cmclics%2Fdomain-rules-override%2B74278%2Cmclics%2Fgmv-predictor%2B52393%2Cmclics%2Foverride-min-seasonality%2B49092&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=57b44c48-d918-4718-a181-ef7677647573&amp;wid=MLA1132090699&amp;sid=search</t>
   </si>
   <si>
     <t>Suplemento En Polvo Hardcore Nutrition Whey Protein Proteínas Sabor Vainilla En Sachet De 1080g</t>
@@ -105,13 +108,13 @@
     <t>40% OFF</t>
   </si>
   <si>
-    <t>https://click1.mercadolibre.com.ar/mclics/clicks/external/MLA/count?a=JxCYIlSibhbWHVsjRpUuZKJ%2BjRuEjdw4J1MuPcOkmKbaUS4uSz7rFZenAszfib87vhjYRz0PETdyDrKTWW2%2FmfFLwur4iMe%2BmkXhxsxCnhQ9Rnmte9IadphOydTAdtZWg6qDumbDPh4U9wVbBXYiPX7iu7lOea%2BHNI1WcCDu9kROxFQmRq1kChWlF9TNj%2FO6R2A5gJEiXQG9CHmeJyYnOpIGLMDRZKczHnYC6k8blO7uaKEItE1NyJZKWU6I53A0hrhcEXSvhDDtxz3GVEAWOZyU7o5muX4eDtfpAhUtMYIoeKSJNlThw9JTgpcCgDnOR1RsWL%2Fx%2FWjOKvywMa1kBV9jFnh3JmGt3koVvZpqkOV0UgC88FbqWYQuebw4mnpQIQ%2FOivCEc4wUpJB14bDD9E9zOxMwT2tvSGD4be%2B4B1U8lehAdpQSOUwglh5fFa807DIvZWWQ3nPga7hm6eaxRFPFhKlaUh2cUEpuRN4i0GTR4w3wQPr0Z79KfFwS2agPOV%2F0MWMQzfU2NKhylQ17XY1NFQPDG7nDnsNH54SEuw5%2BrLgx4f%2BcjcToO6oOWeal%2BqCyrbo%2BK9k6g8cXyRUTVD3O5AuD74vs3Y9xDRxG9EdMkmCcNjJuX2RmFUU0y50q2KC36kfL0B9PX1oChUnPpehZqJyBh1WAXo0bG1qxZ3ikVhr3Nt%2BvAb4aHC6RlzF7E301TMQLF89HR5GXwbG03465%2F9d5UQeaxUVz5YFdkC%2FKsPkoyKJ%2BsGtgHnZVKIvnO9DEK%2F%2B6I9XTxFpcvj8eGbFgsNbWC8jPFv9T5SIvf9DjPTKfgnJiDeEWP9%2FOMC5gx6NviwyORzjxA%2B3wxrCqwaJqKqb%2FdjYjWQZp7vTvzvM%2FtGv6yOtfgU7AV3LD9L7Bs3RGuNxgrNOTsVFrfMRSIxWyck6ioamqbfwhRgVmdTjrP%2FLH%2Ba4IpCk%3D&amp;e=mclics%2Fadvertising-results-augmenter-on%2B15097%2Cmclics%2Fmin-budget-throttling%2B54896%2Cmclics%2Fdiscard-bid-lt-min%2B45363%2Cmclics%2Fdynamic-yield-factor%2B73919%2Cmclics%2Fmore-ads-migration%2B56865%2Cmclics%2Fmax-bid-capped%2B36382%2Cmclics%2Fmax-bid-item-factor%2B23927%2Cmclics%2Fdomain-rules-override%2B74278%2Cmclics%2Fgmv-predictor%2B52393%2Cmclics%2Foverride-min-seasonality%2B49092&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=434de1aa-7e52-46b7-bfd3-877f93b2f905&amp;wid=MLA1905890298&amp;sid=search</t>
+    <t>https://click1.mercadolibre.com.ar/mclics/clicks/external/MLA/count?a=WGtNsAzrxvLZEB52FAnn%2BoAwACSkNcdjHejuOF6O2t9kMZoEcudl%2BhuN2JtLlUTSSXzs1n2SnK6gvXpCbM9kdtujHP9TCHCh%2FTHvVbrq4EJIeTyYq85PddSdj2w3DLvWoRAukUsqC9phwmxaq5cFzS9gVmqKuXzgrJPhK5VUqAtfNMC76fMFOA1pedEjb86sRliExgizT%2B95KWooah8p37AnwC%2B%2FdM1oc7roLxFejAo9AjJUfSesVugxvWS6Yj6aweo%2BmcEd%2Fmw1CXVhDtWyRA8QW9qCiFKmkaiL1mDqbhcTVRpVFVEn5WSgTVyTOwhcRRHXLyudv51eoyn8bW5xsL6EgXEV0wXm%2BbZi%2FImuPX2mNvDimoG56ru%2FuCkcPZgGD60vZaZ9QN971bVfxn1n%2Fmy1Sk%2BPlBJILZ3AFXop8i3mU8R40kDO%2BXpgLjz7wwhfMZxN7zYuMyFtHVcOGuyCoCg00N7erw4weYLJbSHLxhn9i6%2BSIq%2BDZuWIik6bxHZ3P0RA112YRe4RP5f2OUOnx8lY06Rahmdiyf%2BEYTLlcW%2FyO9xrQqhwksnlD0unh5YBCOYc2PZejezoctRZpricxDt2oan7478fI1jo666w9njo92oL8AHrZ70ZEDjdj074JfcydAwUNbNG2MmEpaF3LZ9gNsuGjF9yPvMqBqVfsvpNeYOMscHbWowi3pjbt9lF3qnRMqdYG%2F%2FrXUzxfbaiIhYYAvi0SAZ9gG6wqShn7ZUiVGPoniRTzqFOBY307qcwQnBVX1zj3CFnjbvJF%2F9qBSQnyZAopm%2F7bKNUmv9nVYracX%2BkFIYtA7JO9j42fbnUOorF47zUUJLrd5eDtT5aoANtWRHnP%2Fx%2F0ypU9FuhD2jDmLaGOqpcvBA5QsiV4oBOdwtZxCZC%2FotIX5nInrZ4yrqXLZtoa%2B7ewHueEIcuhXPd792y509NQ%2FAg&amp;e=mclics%2Fadvertising-results-augmenter-on%2B15097%2Cmclics%2Fmin-budget-throttling%2B54896%2Cmclics%2Fdiscard-bid-lt-min%2B45363%2Cmclics%2Fdynamic-yield-factor%2B73919%2Cmclics%2Fmore-ads-migration%2B56865%2Cmclics%2Fmax-bid-capped%2B36382%2Cmclics%2Fmax-bid-item-factor%2B23927%2Cmclics%2Fdomain-rules-override%2B74278%2Cmclics%2Fgmv-predictor%2B52393%2Cmclics%2Foverride-min-seasonality%2B49092&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=57b44c48-d918-4718-a181-ef7677647573&amp;wid=MLA1905890298&amp;sid=search</t>
   </si>
   <si>
     <t>Suplemento en polvo ENA Sport True Made Whey Protein proteínas sabor cookies &amp; cream en pote de 930g</t>
   </si>
   <si>
-    <t>https://www.mercadolibre.com.ar/suplemento-en-polvo-ena-sport-true-made-whey-protein-proteinas-sabor-cookies-cream-en-pote-de-930g/p/MLA14287436#polycard_client=search-nordic&amp;searchVariation=MLA14287436&amp;wid=MLA1116976361&amp;position=22&amp;search_layout=stack&amp;type=product&amp;tracking_id=434de1aa-7e52-46b7-bfd3-877f93b2f905&amp;sid=search</t>
+    <t>https://www.mercadolibre.com.ar/suplemento-en-polvo-ena-sport-true-made-whey-protein-proteinas-sabor-cookies-cream-en-pote-de-930g/p/MLA14287436#polycard_client=search-nordic&amp;searchVariation=MLA14287436&amp;wid=MLA1116976361&amp;position=9&amp;search_layout=stack&amp;type=product&amp;tracking_id=57b44c48-d918-4718-a181-ef7677647573&amp;sid=search</t>
   </si>
   <si>
     <t>True Made Whey Protein 2lbs + Creatina Micronizada 300g Ena Sabor Vainilla</t>
@@ -120,13 +123,13 @@
     <t>20% OFF</t>
   </si>
   <si>
-    <t>https://www.mercadolibre.com.ar/true-made-whey-protein-2lbs-creatina-micronizada-300g-ena-sabor-vainilla/p/MLA28864334#polycard_client=search-nordic&amp;searchVariation=MLA28864334&amp;wid=MLA1897027302&amp;position=3&amp;search_layout=stack&amp;type=product&amp;tracking_id=434de1aa-7e52-46b7-bfd3-877f93b2f905&amp;sid=search</t>
+    <t>https://www.mercadolibre.com.ar/true-made-whey-protein-2lbs-creatina-micronizada-300g-ena-sabor-vainilla/p/MLA28864334#polycard_client=search-nordic&amp;searchVariation=MLA28864334&amp;wid=MLA1897027302&amp;position=10&amp;search_layout=stack&amp;type=product&amp;tracking_id=57b44c48-d918-4718-a181-ef7677647573&amp;sid=search</t>
   </si>
   <si>
     <t>Star Nutrition Whey Protein 2 Lb Sabor Vanilla ice cream Doypack En Polvo</t>
   </si>
   <si>
-    <t>https://www.mercadolibre.com.ar/star-nutrition-whey-protein-2-lb-sabor-vanilla-ice-cream-doypack-en-polvo/p/MLA19545071#polycard_client=search-nordic&amp;searchVariation=MLA19545071&amp;wid=MLA1425719776&amp;position=10&amp;search_layout=stack&amp;type=product&amp;tracking_id=434de1aa-7e52-46b7-bfd3-877f93b2f905&amp;sid=search</t>
+    <t>https://www.mercadolibre.com.ar/star-nutrition-whey-protein-2-lb-sabor-vanilla-ice-cream-doypack-en-polvo/p/MLA19545071#polycard_client=search-nordic&amp;searchVariation=MLA19545071&amp;wid=MLA1425719776&amp;position=4&amp;search_layout=stack&amp;type=product&amp;tracking_id=57b44c48-d918-4718-a181-ef7677647573&amp;sid=search</t>
   </si>
   <si>
     <t>creatina</t>
@@ -135,19 +138,19 @@
     <t>Creatina Star Nutrition 1 Kg Monohidrato Micronizada Sabor Sin sabor</t>
   </si>
   <si>
-    <t>https://click1.mercadolibre.com.ar/mclics/clicks/external/MLA/count?a=%2BUHFnw5sN2bo2o5CZN88gvIJ%2BRBPjXPF5DjqFPY7MPOgiBWTWA31mygrl9HHZfwE6cfp83acxki1WzIUnrkJHs7Zw5K5%2BzUsWpptEdkDiodCpeo8ehx8XPRAV84229HOaYcaeqS7eYPUvlekuNCDyHCxNpOIFMXD5wuVC9pb%2BcfzkI1hHZ%2FK2ht65q057Q%2FhFPGdZc82oqCrYKPLnABL2FWlR2HiJ9I5plcVnyHI1aBteEYnfu5BRSk90jBv%2B%2BExUMxcmXDAq2Lmp8HhRD2zHlcc4xds1GpoWhHZAFafED0PEq7y0GzWs9GUEy97BnZP%2FwZrhQONAOB6ddHJf3kxCdtY5CpdOtDu1EF9p%2B8Fr%2B7TgZOvuETtZ5tcJ%2FT7iRmTARkX2cWJnSWgLQANNCdZ3beXLR9pDio0%2FewNpYOyFFClBNwNKzvoYH8cwIGaGLHuHq6alX4Kj3kjq1A02NjNGZ1Si5ulGCUoY13mKGBckQJfgUWRByCHzyiu0BMNM%2FwuRaAOGYyAxgy9IKho%2Fpbb917GtMe%2BL5zF0a7BOCI6oOS4Ifk9%2B4nelnMIkOmMOo6L0i19SN3JP2IbgE0Us6mQncg5BWcCWEg6hHuldSsK1GRGf6WOv0vA7LfBXZp8BR75d7ExLwVkTptRqaKLMeIfRy5AMKvilPUOoEu9AfSv0uhbnHWX8%2Fsp1pmWBSDywZMa68%2FxFHY8AqUrU47KHvNOpkmo3%2FzcOl%2BqK56mFfOpras77FBG5TkT%2BRGrJoZpwQt7FsBj85LS%2BiwdbOheOwAWJqADm0%2BfSTxSPQftyuir2iPqmSiRx%2BBNC3v29Txo1Na9JaVebq0ALqpCvtdJv4IFYkxiGzTXoowHz6aHwedaiug8fzMBD6Bw3imdeulrpNt55tRve8eLzT%2B3paTm5h0YGg%3D%3D&amp;e=mclics%2Fadvertising-results-augmenter-on%2B15097%2Cmclics%2Fmin-budget-throttling%2B54896%2Cmclics%2Fdiscard-bid-lt-min%2B45363%2Cmclics%2Fdynamic-yield-factor%2B73919%2Cmclics%2Fmore-ads-migration%2B56865%2Cmclics%2Fmax-bid-capped%2B36382%2Cmclics%2Fmax-bid-item-factor%2B23927%2Cmclics%2Fdomain-rules-override%2B74278%2Cmclics%2Fgmv-predictor%2B52393%2Cmclics%2Foverride-min-seasonality%2B49092&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=0d6035e4-891c-492e-98cd-2e4503814c69&amp;wid=MLA1429106527&amp;sid=search</t>
+    <t>https://click1.mercadolibre.com.ar/mclics/clicks/external/MLA/count?a=T2zIXZ6NhUh630gsNPo4uIx2vS%2FrQUMVXbY%2BDUJwiZcs9SiK5IxEB28S31fRxh5xCCTi7DM%2FfkCZVDZQByONzGNKRsXaUYXmcj2natw1Dn4obvKTn8XGFsbdz%2BGlt4P34GKPdA%2BhYr5bgiQrcsBGZqm1zGyQh%2BtVM4%2BTAgKizjNREf6hNxWsLkbzuoZ4Y9u953VdxoV7zpVOly33XJ27R2UeCvOtJNL9g%2F5hkI959DDXcXj4Bu3SVMhPSAJ1AsVelOsox6T5jK1U%2FlIaRRffFpBD3ouy0ihu9%2FX%2Fc8KWqoI87r9s1U%2BTB%2BVFQAUF8zuInFA9OJoq4rRMR12ZGeJD%2BBbhHhXgr5uyHAHR2h1YGGIdThWxXj9B%2B7b0WQ3UG2%2FNNJlNrCYXnjoVM697s6vYCLnLrPfbcV%2ByKL0PKOQFeJ0wBZAW%2B%2FsPRB1g6XjUO8i4XLCU3i6pHa3JNADVEFZ4dKSTqd4A2I9Yjd8bNE6LjyX95LhdX8z7FgQbGja2ToUTolknLpzWBCprDrqoBYq7cXDcC7Nmm82GHYF%2FgiAjGEetQC5oFHDIRtLQlBZADSNbRQwDcxFqI7Hul%2BPsxrhVGZdiNKkFna%2BXgHNJO9SkpOKZx%2BJieq115HWLy1wTEP3X0lww5ORmL32NNJSYFHMnfmX4NWOQm%2FRE7TwMyC2piB4tS18U4qllf4BuCsecZi5XgHVNByDWOkD%2BDQt1sw72%2Fr%2FpYRY4lx9A1%2BJGtoeZUMqgWyNhbMNvpCbCTZHLMArV3EfEZycEKGUumwp3nHv43tHK663BP%2Fns6UbfPEhJNHGS8FaY6aP%2B5bEmMy%2BSjrtNxJvuTMKXtOKKf6iahEVU3dEysNOhhqjaE7hfErMAi%2Bq4Rybk5lF4SF4PCaDxx7ugRLeyf1bK0w4euOueamsz&amp;e=mclics%2Fadvertising-results-augmenter-on%2B15097%2Cmclics%2Fmin-budget-throttling%2B54896%2Cmclics%2Fdiscard-bid-lt-min%2B45363%2Cmclics%2Fdynamic-yield-factor%2B73919%2Cmclics%2Fmore-ads-migration%2B56865%2Cmclics%2Fmax-bid-capped%2B36382%2Cmclics%2Fmax-bid-item-factor%2B23927%2Cmclics%2Fdomain-rules-override%2B74278%2Cmclics%2Fgmv-predictor%2B52393%2Cmclics%2Foverride-min-seasonality%2B49092&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=5d105bfc-84d9-4bd2-92b2-82db1f824132&amp;wid=MLA1429106527&amp;sid=search</t>
   </si>
   <si>
     <t>Creatina Monohidratada Star Nutrition 300 Gr Doypack Vaso Legend 600ml</t>
   </si>
   <si>
-    <t>https://click1.mercadolibre.com.ar/mclics/clicks/external/MLA/count?a=iq82nJq1s5RRE%2Bl3YlP6SIioN%2FXO39eE5YWlI73GLNkEx3C8WGt6xy54%2BDSpdwOwJrnDABSURQSRfoSasJichNxijkPhBPLE1n03IbJMIXTF9zXDjuCD6HhUOVc64Rhl%2FaapG9iWpt2aV8btX9hfk6vGVUQEBsjhQJMUqK6b%2FyIq%2Fmv0%2BrP1KNhrW3Uo8jVdoPCw6SFk9LQxTTvMXHVRN4EvGvDkB1cjNhyBuza3fXhOKLDVna8AnSpgA06sJBDLh25d1JBR3bw7t%2BJn86kFc5d%2Ffh2EW9GM0gd1CQZQG7F3sw3tqpTzMu3hj5XKjlIgEA7woLp2fwZAtRSrPbRHhieiOxgGc5rKXLMFnEtQw2e1Mi7lMkDS5%2FNAX%2FP7M%2FOmiprs%2FAaouQgJS6YPdeEoiOL%2FjUlakpqx%2BsaMVMEGfBJJF7YOjqPRYvBtvR%2FWeNrah9MpOfmCoJFw8nj6T02aK7p7aLDmniPSzA6BnqBBpcNzZb8a5dR%2Bwl%2BR1QhC%2FOOpf9Hp5jROf%2Fjac8frphSbIZDOJMTd7SrLR5V%2FDs%2BrPDGRvo5VwmYc%2BhebsvkmGPDl5lkwUQcA02bQbCrVrj49Dd%2FTqZc8R0LyffprM3dl%2F00PiD7uJMjzUlHDhBOywFVu13vgjpYU2kByr9MGoiQ0SyGbd6xYfcBFnEkuuhlrXd357XPPtifMVW4miXmcE%2Fel1%2FHb3wLQNjK6tJAqyC0mSMVuDLKbh4TpUGqsZARenw1ERkeIQ%2BDFAxdP86GRqg8GdV%2F80WcOidv1LeRy5eoxHj3NhDo5iePchDlGvI3DxG6D%2BlOMNvHCuS1j%2B1TfdyTqV2oIy%2Bg4XVXEFXPHN%2BcUc%2Fv1cq02eua69SvQQqffnWR0FhbghCV4U9YZp6ASxeA07EG%2BHwuw4DxjY0rVUR8HJZ9y&amp;e=mclics%2Fadvertising-results-augmenter-on%2B15097%2Cmclics%2Fmin-budget-throttling%2B54896%2Cmclics%2Fdiscard-bid-lt-min%2B45363%2Cmclics%2Fdynamic-yield-factor%2B73919%2Cmclics%2Fmore-ads-migration%2B56865%2Cmclics%2Fmax-bid-capped%2B36382%2Cmclics%2Fmax-bid-item-factor%2B23927%2Cmclics%2Fdomain-rules-override%2B74278%2Cmclics%2Fgmv-predictor%2B52393%2Cmclics%2Foverride-min-seasonality%2B49092&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=0d6035e4-891c-492e-98cd-2e4503814c69&amp;wid=MLA1894766372&amp;sid=search</t>
+    <t>https://click1.mercadolibre.com.ar/mclics/clicks/external/MLA/count?a=nj6bmtA%2B6ATqiVr1qcNGjk0fM6lY%2BgjHtGt7dcb207A%2BITUPzybdFXmmMGvoac%2FxBDBHWn1QQzNozBb0BYLyGOT4bhSXNU2xFyrb%2BlOJTcrTGH0GayHw8veKRoO9hMrsIAOu8rNYcNUpRs1eS5ltsNZ4tdgyp7siEIEqTKuEFcp9xGMWe%2Bzna%2FBesVlyOsRAT7yC%2B0m68eIMuLKygrtZCcEy61DIEpmce5HblN50RcvgHyKhMQ5EQSjURuxyzM0zBN0WejRefa4KCqgvJJrPyxeuW9mqecO76n3O%2Be0Wgna%2FdIC0L2k9GzjfpRq4XC8D7IlCElFIKwM%2Bu3Twmyfj1PfgqJtMNEAl0bAZizRtEFRZPvAi6kAB0jbadW4h1ZXMX8o8djZ5NDBEiUquhO%2FJroVdhiN86U7QPlavIHh4rEZbrHRSr0e8XAsH2ryf6MHuZQZMZxEKGRW3rC8P0xepKSw14iEkHhroQ6fVqeJLfLXqLCsxlRqjMmOcX0V94lzazMHCJTKkmcSFAYslroaPi1%2FZ0q2R9UOh14ikT6YMxIsjn%2FZarx1TKgZyUbFgZsJn3%2Fux31Scq4a3m9vUbBxmPVf5WU3HYetO%2BucCz4%2FGIzvRhIsi3ilF5p32bJzgYyAOZSGT7GCChv8WVkk7rosL8Amq9oIJXbBYDS9%2FpXqTqfLJiUQpGu41uCgQSiSv1l7pJfzy3XRh4nc8P7QNOZ1OIN9pVfqB8ucIyO%2FSEXY%2BJdWY6gWJOiiBrXWnfIPZolx5rNlmTM8vaNAE9fJ%2B4B3i4fVMhqW2GHWKbt7EgvCh6xFF2b6sTQWVCtdZ2kLUIH%2FTDD3dn799LSsjnqtqf8KwxdmYKaGGUuu0TPgOdGIU56LQrnXLBF3eCBRF0ORMPWMdwB2fdtMo5JiS6nc0h0YRG2Q%3D&amp;e=mclics%2Fadvertising-results-augmenter-on%2B15097%2Cmclics%2Fmin-budget-throttling%2B54896%2Cmclics%2Fdiscard-bid-lt-min%2B45363%2Cmclics%2Fdynamic-yield-factor%2B73919%2Cmclics%2Fmore-ads-migration%2B56865%2Cmclics%2Fmax-bid-capped%2B36382%2Cmclics%2Fmax-bid-item-factor%2B23927%2Cmclics%2Fdomain-rules-override%2B74278%2Cmclics%2Fgmv-predictor%2B52393%2Cmclics%2Foverride-min-seasonality%2B49092&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=5d105bfc-84d9-4bd2-92b2-82db1f824132&amp;wid=MLA1894766372&amp;sid=search</t>
   </si>
   <si>
     <t>Creatina Monohidrato 500 Gr Gentech Sin Tacc Sabor Neutro</t>
   </si>
   <si>
-    <t>https://www.mercadolibre.com.ar/creatina-monohidrato-500-gr-gentech-sin-tacc-sabor-neutro/p/MLA23451289#polycard_client=search-nordic&amp;searchVariation=MLA23451289&amp;wid=MLA1757348654&amp;position=12&amp;search_layout=stack&amp;type=product&amp;tracking_id=0d6035e4-891c-492e-98cd-2e4503814c69&amp;sid=search</t>
+    <t>https://www.mercadolibre.com.ar/creatina-monohidrato-500-gr-gentech-sin-tacc-sabor-neutro/p/MLA23451289#polycard_client=search-nordic&amp;searchVariation=MLA23451289&amp;wid=MLA1757348654&amp;position=4&amp;search_layout=stack&amp;type=product&amp;tracking_id=5d105bfc-84d9-4bd2-92b2-82db1f824132&amp;sid=search</t>
   </si>
   <si>
     <t>Suplemento en polvo ENA Sport Creatina micronizada 100% Pura en Doypack de 300g sabor neutro</t>
@@ -156,43 +159,43 @@
     <t>8% OFF</t>
   </si>
   <si>
-    <t>https://www.mercadolibre.com.ar/suplemento-en-polvo-ena-sport-creatina-micronizada-100-pura-en-doypack-de-300g-sabor-neutro/p/MLA18907230#polycard_client=search-nordic&amp;searchVariation=MLA18907230&amp;wid=MLA1232452267&amp;position=9&amp;search_layout=stack&amp;type=product&amp;tracking_id=0d6035e4-891c-492e-98cd-2e4503814c69&amp;sid=search</t>
+    <t>https://www.mercadolibre.com.ar/suplemento-en-polvo-ena-sport-creatina-micronizada-100-pura-en-doypack-de-300g-sabor-neutro/p/MLA18907230#polycard_client=search-nordic&amp;searchVariation=MLA18907230&amp;wid=MLA1232452267&amp;position=5&amp;search_layout=stack&amp;type=product&amp;tracking_id=5d105bfc-84d9-4bd2-92b2-82db1f824132&amp;sid=search</t>
   </si>
   <si>
     <t>Creatina Monohidratada Star Nutrition 300g Doypack</t>
   </si>
   <si>
-    <t>https://www.mercadolibre.com.ar/creatina-monohidratada-star-nutrition-300g-doypack/p/MLA37675709#polycard_client=search-nordic&amp;searchVariation=MLA37675709&amp;wid=MLA1815201134&amp;position=5&amp;search_layout=stack&amp;type=product&amp;tracking_id=0d6035e4-891c-492e-98cd-2e4503814c69&amp;sid=search</t>
+    <t>https://www.mercadolibre.com.ar/creatina-monohidratada-star-nutrition-300g-doypack/p/MLA37675709#polycard_client=search-nordic&amp;searchVariation=MLA37675709&amp;wid=MLA1815201134&amp;position=8&amp;search_layout=stack&amp;type=product&amp;tracking_id=5d105bfc-84d9-4bd2-92b2-82db1f824132&amp;sid=search</t>
   </si>
   <si>
     <t>Suplemento En Polvo Star Nutrition Creatine Monohydrate Pote 300g Vaso Legend Nutrition 600ml</t>
   </si>
   <si>
-    <t>https://click1.mercadolibre.com.ar/mclics/clicks/external/MLA/count?a=zC6OULt17o5aM4hNWFrLN7UDGHGzdgqErq3BpwGfUL3n08uA8WInHKyuZK82qJs4SOciTvz6XDb9Klv1sVsWdX7l%2BFNeiCt91ZvxQdJULDHAv1kLCRGxt8%2BlBWvOgvcGuWd2kAcLKGtHFUtHkPORn2FD7XUCnAHOi57lUK6gxLFdi0ZRqrzzXhC6v2ZTbQKX5oceueBV7IOVfFF6yVV1zCNQPwerYyMHKNNdLefmBbek4WMH3z2Z2cBFoPHufiGetC9UZjYY35CAO9fAtlnl9PfKqvQDvt3cjh%2BUotKi5jGW0ar3GE7OQEPEkTopK3Zk4FgNbzlvlck1zQtBjh8SkMN08QHbkehS9I6%2FGxOyy739ZemVyi11I3TFxxXT%2FGsOIAAWe%2B4%2FEbXIJ30WyK9TZVvy86B5PvpRhXfZFI4e0MyMQgEWhVFBUElfTjR4IJHDqoysY6itFpB4r3zJ%2B0CAzspUeqKAMuJhl1S2fVgwWmEpGZDm%2BLQ%2BOu1qSvwSD0a5PdnHPQGA3sVQhEXm3ykGQ7JWe2ZRglSEol18SvPlgkT4V1lgm7PfLRq94HbSmjr72CoRt4MsI52PwqTKl%2Bk7peTsuVXD3D0L%2BCst8RZ2LVQIh8okRVFzdBUjbT4%2FA2QkPKgdNg2G5e4AhSuHSU%2B%2FczXfq53ztJ9lq0WbStNtOFIIze2wXNElRd1ByKphzUBiwU5NQS4YADNtGJPKUQ4NaNj2SrrK6cseexN3zo2%2F11s%2FbovR0N4oeIfDmtZZHr1VIlvv2DdHgJ%2BHEZlwRCF3dAKOpyfH0hy34mSO5jYfD%2FrTLi%2Fr9skIQMW0UnKF2buI32a83SgB7pzjhBXKXxA%2FQoXIXQTW320s0gCTtT%2BBmwROhBBCrZEkQYFmJkxcRsY8U6bU2MgRqYzIWlKfWOaiRB%2Br7W58vYUD1K8dhX19kkovmhn9vzOpqg%3D%3D&amp;e=mclics%2Fadvertising-results-augmenter-on%2B15097%2Cmclics%2Fmin-budget-throttling%2B54896%2Cmclics%2Fdiscard-bid-lt-min%2B45363%2Cmclics%2Fdynamic-yield-factor%2B73919%2Cmclics%2Fmore-ads-migration%2B56865%2Cmclics%2Fmax-bid-capped%2B36382%2Cmclics%2Fmax-bid-item-factor%2B23927%2Cmclics%2Fdomain-rules-override%2B74278%2Cmclics%2Fgmv-predictor%2B52393%2Cmclics%2Foverride-min-seasonality%2B49092&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=0d6035e4-891c-492e-98cd-2e4503814c69&amp;wid=MLA1913522990&amp;sid=search</t>
-  </si>
-  <si>
-    <t>Creatine Monohydrate 100% Pure 500 Gramos - Animal</t>
-  </si>
-  <si>
-    <t>https://click1.mercadolibre.com.ar/mclics/clicks/external/MLA/count?a=IKOP6S26ARw4QnjwrvxJiepwTIOxfHPjqY%2F8X7uA38rtaKU48ZwbEKK3puQ5hAGu%2F%2Be2656SuVQll85MFmFCQauvcCC9wODqZe8Zn8TAp7bC8IUXM7CgPpwFo3lj1SkRPO5zP4o83OlFXO0gSoghgIkO%2F6HDWZh7PlZdYNWjkoKhS6JlANoarFsPCm2K89SwLG5OAkLOfK0FXYg6XOjBgiXexTEUst%2FnYakxkwlSddqYwV%2FYl2S5RkBPoPwFC6h%2FyP0wAMSs0k05KMagvg%2F0APH0rtwt77Pf%2FoR3GRM26VYYmYfNVOS3vi7Jlc4C6Ynx7ScYO%2FLh5iS05KI0tjAGcsuis38tGROKtWmD3TwRlYGukCGFlVsFDnIK47KE75kg3sMKkMVjQ%2FcAm8ocbNnUeBV9F%2BesPbh8WBsproCpdrwk9nN5s5W2Qv2jNLDnPSKHZkjlMG%2F5hI5tgcl2M7wzbojv%2FPXeZoP1DkR%2FIMSUKB3%2B66yxCauHeo7pycdAjgnnxFYZg28FDmBMqAZ33oEXLLSUzHGWSRZMqzReIYnIIaM10YgKbmcQLWzQF%2B9bD4E2hcHtoUUqUAwxTBCEkIxmGkAXu0d0PD1JVdGmXa99X47Q%2Fo3PkgwL%2B3vEqaAQ%2BlrIthJ%2BAXMgQVkxFXTani8j%2BTNxt3VJyzZYznRdDhcwqigRe9yNA%2Fvxd2rWwh4qh0cPRrxJIWD6xWm%2B3Kc7LBnmgRgfnx8sxVFgnDsBi4k%2BritBZPNvVtCED5k6TV7MuJZLuIpJdP4uq6q53IsR6lTBBiy4sdCTkoqFcsGbc9wRfGZ7DqWzIHz%2BXGEZMEtO4aIzOSpGzpxwTZ9DGQoG34AotPNFloHJm2tkhLb2QvYXY1j3SPDdV8VjCA%3D%3D&amp;e=mclics%2Fadvertising-results-augmenter-on%2B15097%2Cmclics%2Fmin-budget-throttling%2B54896%2Cmclics%2Fdiscard-bid-lt-min%2B45363%2Cmclics%2Fdynamic-yield-factor%2B73919%2Cmclics%2Fmore-ads-migration%2B56865%2Cmclics%2Fmax-bid-capped%2B36382%2Cmclics%2Fmax-bid-item-factor%2B23927%2Cmclics%2Fdomain-rules-override%2B74278%2Cmclics%2Fgmv-predictor%2B52393%2Cmclics%2Foverride-min-seasonality%2B49092&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=0d6035e4-891c-492e-98cd-2e4503814c69&amp;wid=MLA2006037468&amp;sid=search</t>
+    <t>https://click1.mercadolibre.com.ar/mclics/clicks/external/MLA/count?a=6vO%2BBeBDOuDVZ3vC07iySKxbHdUT%2BHV3H9HSml6gLTiFJ4XGAto7DN005L0jC59Y4nAyu0rYmNa406kmY%2BziCW79rvh3p6nrL5VbsdgYj47vge9zJTTq4zAfkpXP%2FrEwMuiJ3wycNPZuGIlKG5Am9NwiANFicnGbYdL3loY6aVgeXwJ6cmocAiMZCVm24hhEZb4pRQuKUDseW8wZLJdLViCOLujxgBZywasOQddkuhA1%2BwSaVUd6d9FObx%2B6eKcDXtOqr9eYS7Ebr1iWbjEQM8X5vguToJoO1Yl7mht2TwlID7P3%2BmhtXgDm6JXT5%2F%2BJyJlVF1qIZSF1XQrDlCR7FIXdpUcPhnJOSALvmfuPtRVe9lfMdG4aFlwxgy3YFg1%2BMYwS4kgWRIRKuJCxFbLl%2F3NtrWJH%2BXmU7%2B9ljokO8NA2gso%2Fn3tZ8r7%2BhZ6s7z%2Bq4rxWiWgkyWKPbVbRxh2a6TYhEhHX9FIXLDnz99d2HoKeF3K6xpe6ev92i8l1Ta2B78WvKGHdoqWsCrmWrZCQ0DxGJWuo64hPpwjhq6m3v4DWd4Ve7lXLd9NSpGQ0VzZS42F%2B1FmG%2BA%2B4%2BNIZWppJ4WBH0HrrDJpFiwAmho1B2f1v17ABm8xfDEdLIFA5ltvLJww7bfNM5x4HBhcwXNyBg4AHSemmja9QsbzPNLRINPLwhRs11ifc%2FHFc28U8gkgJWLhRyWzTA8QMv%2BsoAMmYWKIMqxanWKmp0mgDvs1iQe%2Ft2DerjK06avQJKxmo5Sbgf0zuEIdDzNqWGS1yNPvzwNBUd5NATlCA%2FtXp8XllofhNo%2F3%2BSz%2B7%2BYgAG7dtjU56NtJIQOE0dqw3FpYs50u6yKceENelLlCwubr49oBM0nCxJkw4m1dHZPTZZplkCD%2Fcx3fv9OYqyuHEKg2ESgx%2BfuV4juwy6ozK1oUQ0Xqfw6E101Me1%2BfM&amp;e=mclics%2Fadvertising-results-augmenter-on%2B15097%2Cmclics%2Fmin-budget-throttling%2B54896%2Cmclics%2Fdiscard-bid-lt-min%2B45363%2Cmclics%2Fdynamic-yield-factor%2B73919%2Cmclics%2Fmore-ads-migration%2B56865%2Cmclics%2Fmax-bid-capped%2B36382%2Cmclics%2Fmax-bid-item-factor%2B23927%2Cmclics%2Fdomain-rules-override%2B74278%2Cmclics%2Fgmv-predictor%2B52393%2Cmclics%2Foverride-min-seasonality%2B49092&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=5d105bfc-84d9-4bd2-92b2-82db1f824132&amp;wid=MLA1913522990&amp;sid=search</t>
+  </si>
+  <si>
+    <t>Suplemento en polvo Hardcore Nutrition Creatina sabor frutilla x 1kg</t>
+  </si>
+  <si>
+    <t>45% OFF</t>
+  </si>
+  <si>
+    <t>https://click1.mercadolibre.com.ar/mclics/clicks/external/MLA/count?a=awQvOkFtS%2B2NRbpWCqabp06BCUxbEL2oXgH3BoEtdPOmrOOniiNN6Vo8R%2BJpLKwGvAQ7JCcVs2o8Yjo6LHOxJmykSxSasJHDt0y%2FriIzsNJr7vTDGi6qpl66R5TTkY9rk8HzsxqCXLQSiYO11P9VyiWsgjxz8jgGlZ9QXQjWVGrhQcAmU3%2BLQxyPzApsGL8FP%2Bmel5plh8B0HmvVx7fMXd6Lw%2FxtEqhuEVjKpvEN9pBNJHECrtXuV9Sui0uEAiyj9Prt%2B1BH9GxTJRTrPiXdvIsDDkeobedcbtGMPLtMWwNKJFDIK36YSMrogxt87pxw9uRUGwtmWSqdUsV0ySzXpm%2FCLGfsdGf%2Bd1OwJ1JtNVhdTGnoM195c652io5bg%2BaqVFCBFvjNbiy75ElhNR1xMT1haIwU6rdol%2FinReMhNicRQp%2FKv149OC57yyuWEDapzYtdX7NRGkZOhCm2b6YEc2xYbja%2Fg2G8hRIXAFonIx2o4dl3Si3JdbsGELLQz4GpkJNYts%2BqMCjVY6xTLjDKwz05osOJLjD51Ih7cXTorwMvSosPvdclK7RuNluFWUMjHFJy3gy8acqzlapSEtLsyozD5WPYtlO7X8G%2BjcZpg8kS1uEKk1GOQryaHxUWllD55%2F0kH446Hx3SPRD1eJm24wbm%2BQ%2BoRzHVWgsf7Egz1nRPWiQFUBLBhD0nPwu8PVdBGPD1m4Y6s9ZPkfROsGkwn7za0XU0OyRGfvXFte%2BuXnvKB2Re1FUnnrxrdyW8pbgpLGzmhdW4EDdYOMoU9YUqaSK6MtBsOGrCXqCUqUB9Gz75pdwYRr6cfKQpa%2Bz2RrNlQxFZHlj6lgWt%2BBBVn3KXy7%2F4ry9Aov0t9aPvpDy1U%2FWBYWmHsXL79zbxXCJP0VvKuKTGeWfrkNAbxb%2F9I2Y%3D&amp;e=mclics%2Fadvertising-results-augmenter-on%2B15097%2Cmclics%2Fmin-budget-throttling%2B54896%2Cmclics%2Fdiscard-bid-lt-min%2B45363%2Cmclics%2Fdynamic-yield-factor%2B73919%2Cmclics%2Fmore-ads-migration%2B56865%2Cmclics%2Fmax-bid-capped%2B36382%2Cmclics%2Fmax-bid-item-factor%2B23927%2Cmclics%2Fdomain-rules-override%2B74278%2Cmclics%2Fgmv-predictor%2B52393%2Cmclics%2Foverride-min-seasonality%2B49092&amp;rb=x#polycard_client=search-nordic&amp;tracking_id=5d105bfc-84d9-4bd2-92b2-82db1f824132&amp;wid=MLA1138355031&amp;sid=search</t>
   </si>
   <si>
     <t>Suplemento En Polvo Star Nutrition Creatine Monohydrate En Pote De 300g Sin sabor</t>
   </si>
   <si>
-    <t>0% OFF</t>
-  </si>
-  <si>
-    <t>https://www.mercadolibre.com.ar/suplemento-en-polvo-star-nutrition-creatine-monohydrate-en-pote-de-300g-sin-sabor/p/MLA13283558#polycard_client=search-nordic&amp;searchVariation=MLA13283558&amp;wid=MLA1145210170&amp;position=4&amp;search_layout=stack&amp;type=product&amp;tracking_id=0d6035e4-891c-492e-98cd-2e4503814c69&amp;sid=search</t>
-  </si>
-  <si>
-    <t>https://www.mercadolibre.com.ar/creatina-monohidratada-star-nutrition-300-gr-doypack-vaso-legend-600ml/p/MLA39936702#polycard_client=search-nordic&amp;searchVariation=MLA39936702&amp;wid=MLA1894766372&amp;position=8&amp;search_layout=stack&amp;type=product&amp;tracking_id=0d6035e4-891c-492e-98cd-2e4503814c69&amp;sid=search</t>
+    <t>https://www.mercadolibre.com.ar/suplemento-en-polvo-star-nutrition-creatine-monohydrate-en-pote-de-300g-sin-sabor/p/MLA13283558#polycard_client=search-nordic&amp;searchVariation=MLA13283558&amp;wid=MLA1137239021&amp;position=9&amp;search_layout=stack&amp;type=product&amp;tracking_id=5d105bfc-84d9-4bd2-92b2-82db1f824132&amp;sid=search</t>
+  </si>
+  <si>
+    <t>https://www.mercadolibre.com.ar/creatina-monohidratada-star-nutrition-300-gr-doypack-vaso-legend-600ml/p/MLA39936702#polycard_client=search-nordic&amp;searchVariation=MLA39936702&amp;wid=MLA1894766372&amp;position=10&amp;search_layout=stack&amp;type=product&amp;tracking_id=5d105bfc-84d9-4bd2-92b2-82db1f824132&amp;sid=search</t>
   </si>
   <si>
     <t>ENA Sport Monohidrato de Creatina Micronizada 300 g Polvo Doypack Fruit punch</t>
   </si>
   <si>
-    <t>https://www.mercadolibre.com.ar/ena-sport-monohidrato-de-creatina-micronizada-300-g-polvo-doypack-fruit-punch/p/MLA18907231#polycard_client=search-nordic&amp;searchVariation=MLA18907231&amp;wid=MLA1142841367&amp;position=3&amp;search_layout=stack&amp;type=product&amp;tracking_id=0d6035e4-891c-492e-98cd-2e4503814c69&amp;sid=search</t>
+    <t>https://www.mercadolibre.com.ar/ena-sport-monohidrato-de-creatina-micronizada-300-g-polvo-doypack-fruit-punch/p/MLA18907231#polycard_client=search-nordic&amp;searchVariation=MLA18907231&amp;wid=MLA1142841367&amp;position=11&amp;search_layout=stack&amp;type=product&amp;tracking_id=5d105bfc-84d9-4bd2-92b2-82db1f824132&amp;sid=search</t>
   </si>
 </sst>
 </file>
@@ -574,7 +577,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34974047-1F2B-43DB-BFEC-0B55E7D130E2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3156BFCD-10BE-4E75-B929-062C09A94D74}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -612,7 +615,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="4">
-        <v>35468</v>
+        <v>38087</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>8</v>
@@ -632,7 +635,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="4">
-        <v>38087</v>
+        <v>107834</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>8</v>
@@ -689,16 +692,16 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D6" s="4">
-        <v>35493</v>
+        <v>35468</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -709,16 +712,16 @@
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="4">
-        <v>107834</v>
+        <v>38087</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -729,16 +732,16 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" s="4">
         <v>12000</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -749,7 +752,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D9" s="4">
         <v>38675</v>
@@ -758,7 +761,7 @@
         <v>13</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -769,16 +772,16 @@
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" s="4">
         <v>65200</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -789,7 +792,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" s="4">
         <v>35469</v>
@@ -798,7 +801,7 @@
         <v>8</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -806,10 +809,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12" s="4">
         <v>89915</v>
@@ -818,7 +821,7 @@
         <v>8</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -826,19 +829,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D13" s="4">
         <v>31086</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -846,10 +849,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D14" s="4">
         <v>34000</v>
@@ -858,7 +861,7 @@
         <v>13</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -866,19 +869,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D15" s="4">
         <v>33120</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -886,19 +889,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D16" s="4">
         <v>34196</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -906,10 +909,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D17" s="4">
         <v>34359</v>
@@ -918,7 +921,7 @@
         <v>8</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -926,19 +929,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D18" s="4">
-        <v>47031</v>
+        <v>21760</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -946,19 +949,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D19" s="4">
         <v>34359</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -966,19 +969,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D20" s="4">
         <v>31086</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -986,19 +989,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D21" s="4">
         <v>33000</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>